<commit_message>
added the data for visualisation. updated the results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinivassuri/Documents/CIS545-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97B1610-90A3-224A-A448-DB70DF4690CF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA55AEB-F278-3841-A2E2-382498710F29}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" xr2:uid="{A8420581-E169-9448-9380-F84C410DDE12}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" activeTab="4" xr2:uid="{A8420581-E169-9448-9380-F84C410DDE12}"/>
   </bookViews>
   <sheets>
     <sheet name="PCA-30-Corpus" sheetId="1" r:id="rId1"/>
     <sheet name="PCA_30_Polarity" sheetId="2" r:id="rId2"/>
+    <sheet name="PCA_100_corpus" sheetId="3" r:id="rId3"/>
+    <sheet name="PCA_100_Polarity" sheetId="4" r:id="rId4"/>
+    <sheet name="PCA-300-Polarity" sheetId="5" r:id="rId5"/>
+    <sheet name="PCA-300-Corpus" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t xml:space="preserve"> ngram</t>
   </si>
@@ -83,6 +87,48 @@
   </si>
   <si>
     <t>Corpus Sentiment</t>
+  </si>
+  <si>
+    <t>Observations : Classification is better to be performed on 1 gram than bi/tri grams</t>
+  </si>
+  <si>
+    <t>Trigram accuracy is very bad</t>
+  </si>
+  <si>
+    <t>Ngram</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> svm_train</t>
+  </si>
+  <si>
+    <t>svm_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dt_train</t>
+  </si>
+  <si>
+    <t>rf_train</t>
+  </si>
+  <si>
+    <t>1gram</t>
+  </si>
+  <si>
+    <t>2gram</t>
+  </si>
+  <si>
+    <t>3gram</t>
+  </si>
+  <si>
+    <t>logreg_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> adaboost_test</t>
+  </si>
+  <si>
+    <t>ngram</t>
+  </si>
+  <si>
+    <t>ngrams</t>
   </si>
 </sst>
 </file>
@@ -148,10 +194,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -472,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAAABF8-D564-DF4E-BE3F-9EB109A762A3}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,10 +599,10 @@
       <c r="I2" s="1">
         <v>0.54465799999999998</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="3">
         <v>0.66095499999999996</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="3">
         <v>0.61738300000000002</v>
       </c>
       <c r="L2" s="1">
@@ -643,6 +692,16 @@
       </c>
       <c r="M4" s="1">
         <v>0.47283700000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -671,6 +730,414 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4238A3A5-17B3-204E-82BC-0267EA391AAA}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.60684700000000003</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.60514100000000004</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.52404499999999998</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.51971999999999996</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.60079499999999997</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.59860199999999997</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.59954300000000005</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.59307200000000004</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.69508700000000001</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.65692799999999996</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.60746199999999995</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.60267099999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.53445600000000004</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.53599699999999995</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.50204000000000004</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.50560000000000005</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.528277</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.53102400000000005</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.56964300000000001</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.56406500000000004</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.62340300000000004</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.59536699999999998</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.56852999999999998</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.56027400000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.49860900000000002</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.49867800000000001</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.49233700000000002</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.49179200000000001</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.498446</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.49867800000000001</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.52354699999999998</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.52222500000000005</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.53935999999999995</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.52876299999999998</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.52179600000000004</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.52187700000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC21AE8F-643E-3D4A-88A1-D8E7ED901545}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B4D204-AE22-5A49-B8B8-3DB8249AEEDF}">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.67854199999999998</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.68189999999999995</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.56522600000000001</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.56048299999999995</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.67477500000000001</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.67817899999999998</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.62526999999999999</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.61794000000000004</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.743838</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.71035099999999995</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.65472900000000001</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.65358899999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.57621699999999998</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.575021</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.53829400000000005</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.53575399999999995</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.57169499999999995</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.57199500000000003</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.57060500000000003</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.56566499999999997</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.64034100000000005</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.60434100000000002</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.58527099999999999</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.57481199999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.51828300000000005</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.51346000000000003</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.50244599999999995</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.49627900000000003</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.51783100000000004</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.512521</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.51711200000000002</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.51196399999999997</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.54228200000000004</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.52806799999999998</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.52515800000000001</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.51999899999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8F8A95-262D-CF43-8161-31044A042CD2}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D2DB51-3C1C-2842-A2DC-2E35434B9C05}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
added polarity with 300 pca
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinivassuri/Documents/CIS545-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA55AEB-F278-3841-A2E2-382498710F29}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7AADF5-A6D5-6B4D-A701-234410DA1466}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" activeTab="4" xr2:uid="{A8420581-E169-9448-9380-F84C410DDE12}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
   <si>
     <t xml:space="preserve"> ngram</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>ngrams</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nb_train</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> adaboost_train</t>
   </si>
 </sst>
 </file>
@@ -1103,32 +1109,176 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8F8A95-262D-CF43-8161-31044A042CD2}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="J2" sqref="J2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="46" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" s="1">
+        <v>0.76173900000000005</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.75984300000000005</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.58704500000000004</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.58754200000000001</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.76102000000000003</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.76074699999999995</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.634405</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.63171299999999997</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.776868</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.75904300000000002</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.67621200000000004</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.67383099999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>0.60944399999999999</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.60322799999999999</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.55218299999999998</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.55161400000000005</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.60821499999999995</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.60246200000000005</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.57006100000000004</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.56510899999999997</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.63682799999999995</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.60987100000000005</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.589202</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.582986</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.53217199999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.52288500000000004</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.51551199999999997</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.50866</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.53228799999999998</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.52316399999999996</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.51734400000000003</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.51196399999999997</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.54363899999999998</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.52660700000000005</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.53046800000000005</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.52097199999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushed with 300 components pca
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinivassuri/Documents/CIS545-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7AADF5-A6D5-6B4D-A701-234410DA1466}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF6946E-D3EC-D040-A789-F5D863BE3972}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" activeTab="4" xr2:uid="{A8420581-E169-9448-9380-F84C410DDE12}"/>
   </bookViews>
@@ -1112,7 +1112,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K2"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated the results for the classifiers
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinivassuri/Documents/CIS545-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF6946E-D3EC-D040-A789-F5D863BE3972}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E8C113-5085-0C42-A0E7-7EE408FFF1BE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" activeTab="4" xr2:uid="{A8420581-E169-9448-9380-F84C410DDE12}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" activeTab="5" xr2:uid="{A8420581-E169-9448-9380-F84C410DDE12}"/>
   </bookViews>
   <sheets>
     <sheet name="PCA-30-Corpus" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
   <si>
     <t xml:space="preserve"> ngram</t>
   </si>
@@ -1111,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8F8A95-262D-CF43-8161-31044A042CD2}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1288,12 +1288,179 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D2DB51-3C1C-2842-A2DC-2E35434B9C05}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.69544600000000001</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.69476899999999997</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.54695400000000005</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.549597</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.69201400000000002</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.69125599999999998</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.55613699999999999</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.54657100000000003</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.71076099999999998</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.68569100000000005</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.59662199999999999</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.59303700000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.55484999999999995</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.55728299999999997</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.51846899999999996</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.52257200000000004</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.55385300000000004</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.55655299999999996</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.53728500000000001</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.53923200000000004</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.589005</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.56747400000000003</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.53417800000000004</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.53787600000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.48330499999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.47436699999999998</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.47007700000000002</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.46372400000000003</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.48258600000000001</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.47429700000000002</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.48403600000000002</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.47067999999999999</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.49601200000000001</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.477219</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.47928199999999999</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.470611</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added all the resultts
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinivassuri/Documents/CIS545-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E8C113-5085-0C42-A0E7-7EE408FFF1BE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2742403-F442-B44B-9B0E-B92AEDF49057}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" activeTab="5" xr2:uid="{A8420581-E169-9448-9380-F84C410DDE12}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" activeTab="2" xr2:uid="{A8420581-E169-9448-9380-F84C410DDE12}"/>
   </bookViews>
   <sheets>
     <sheet name="PCA-30-Corpus" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="35">
   <si>
     <t xml:space="preserve"> ngram</t>
   </si>
@@ -918,12 +918,179 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC21AE8F-643E-3D4A-88A1-D8E7ED901545}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.64399300000000004</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.63981600000000005</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.54246799999999995</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.53738900000000001</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.63775599999999999</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.63446000000000002</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.55946399999999996</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.558083</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.68155699999999997</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.65675399999999995</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.59143900000000005</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.58886300000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.52627100000000004</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.52681599999999995</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.50060300000000002</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.50351299999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.524509</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.52392899999999998</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.53748200000000002</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.52980700000000003</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.57601999999999998</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.55585700000000005</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.53547699999999998</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.53119799999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.469057</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.468802</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.45826299999999998</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.45972499999999999</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.46887099999999998</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.468663</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.47992000000000001</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.47808800000000001</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.49047000000000002</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.48100999999999999</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.47603600000000001</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.47579300000000002</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1290,7 +1457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D2DB51-3C1C-2842-A2DC-2E35434B9C05}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
results along with 300word vec
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinivassuri/Documents/CIS545-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2742403-F442-B44B-9B0E-B92AEDF49057}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54ADA22C-301F-A642-BAEC-1C2FA72254D7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" activeTab="2" xr2:uid="{A8420581-E169-9448-9380-F84C410DDE12}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" activeTab="6" xr2:uid="{A8420581-E169-9448-9380-F84C410DDE12}"/>
   </bookViews>
   <sheets>
     <sheet name="PCA-30-Corpus" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="PCA_100_Polarity" sheetId="4" r:id="rId4"/>
     <sheet name="PCA-300-Polarity" sheetId="5" r:id="rId5"/>
     <sheet name="PCA-300-Corpus" sheetId="6" r:id="rId6"/>
+    <sheet name="WordVec300" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="35">
   <si>
     <t xml:space="preserve"> ngram</t>
   </si>
@@ -528,7 +529,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -920,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC21AE8F-643E-3D4A-88A1-D8E7ED901545}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1279,7 +1280,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1630,4 +1631,101 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9AFB1A-1D9D-964C-B0B6-CF44C4D46B52}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.73259200000000002</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.72847099999999998</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.60822699999999996</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.60493200000000003</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.73077199999999998</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.72586300000000004</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.61246999999999996</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.59884499999999996</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.79233399999999998</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.73514900000000005</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.62022600000000006</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.61654799999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>